<commit_message>
Mudança nome das sheets
</commit_message>
<xml_diff>
--- a/Suporte_Relatorio.xlsx
+++ b/Suporte_Relatorio.xlsx
@@ -5,29 +5,26 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ekhofo.sharepoint.com/Shared Documents/Dados/Gestão/Benny/Relatório Mensal - Teste CD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ekhofo-my.sharepoint.com/personal/rafael_astolfi_ekhofo_com/Documents/Desktop/relatorio_mensal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="8_{99956F94-DCAB-454E-864B-055737CC37DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1110582C-0352-4642-9A27-A8EDC68ABD74}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="8_{99956F94-DCAB-454E-864B-055737CC37DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7984F64E-BCD3-460D-9818-07A3ACF8A2C7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="5" xr2:uid="{D83840C6-8BB1-4146-989F-64A28F905889}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{D83840C6-8BB1-4146-989F-64A28F905889}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
     <sheet name="carteira_ekho_onshore" sheetId="13" r:id="rId2"/>
     <sheet name="carteira_ekho_offshore" sheetId="14" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
-    <sheet name="clients_on_off" sheetId="10" r:id="rId5"/>
-    <sheet name="clients_onshore" sheetId="11" r:id="rId6"/>
-    <sheet name="classes(backup)" sheetId="12" r:id="rId7"/>
-    <sheet name="clients_on_off (2)" sheetId="15" r:id="rId8"/>
-    <sheet name="clients_onshore (2)" sheetId="16" r:id="rId9"/>
+    <sheet name="classes(backup)" sheetId="12" r:id="rId5"/>
+    <sheet name="clients_on_off" sheetId="15" r:id="rId6"/>
+    <sheet name="clients_onshore" sheetId="16" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classes!$A$1:$E$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'classes(backup)'!$A$1:$E$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">clients_on_off!$A$1:$C$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'clients_on_off (2)'!$A$1:$C$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'classes(backup)'!$A$1:$E$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">clients_on_off!$A$1:$C$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet2!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -51,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="114">
   <si>
     <t>Alternativos</t>
   </si>
@@ -400,10 +397,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -530,7 +527,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -543,7 +540,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -559,13 +556,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -573,7 +570,7 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+      <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -2617,163 +2614,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B5D382-D8EA-44BA-BECC-FE54A135637F}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B12" sqref="B12"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="49.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1016</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="24">
-        <v>45198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="3">
-        <v>2016</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="24">
-        <v>45383</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1017</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="24">
-        <v>45198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="3">
-        <v>2017</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="24">
-        <v>45323</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{443D88F5-9A01-4293-B5E9-8ED0BCA7DE7F}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B12" sqref="B12"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="24" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="3">
-        <v>22365</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="24">
-        <v>45195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1010</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="24">
-        <v>45373</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A0DD4C-F195-4C71-8353-E46AFFEBC95A}">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -3090,7 +2930,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDD9564B-AAE5-4B8B-854B-0D27C6086BCC}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -3714,11 +3554,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A787322A-5B17-4E1F-B960-30BFFEBBD83A}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B12" sqref="B12"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3:D3"/>
@@ -4046,15 +3886,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010029DFE9A47EDBBA4C9642CECEC7AB5212" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8f2c6ae4a50a8b148bb7565151eccd01">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="685e8f7b-ce85-439b-962f-3948db74e463" xmlns:ns3="9968dc3e-a1f3-41f5-b998-9e98f3d19f76" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="182854d0ea7c01653fabf173265a5b93" ns2:_="" ns3:_="">
     <xsd:import namespace="685e8f7b-ce85-439b-962f-3948db74e463"/>
@@ -4289,6 +4120,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4309,14 +4149,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11E769B2-782A-4CC9-89C8-BE475949AFF9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BA1717C-B4B5-41B3-9092-3632DE0736F1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4331,6 +4163,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11E769B2-782A-4CC9-89C8-BE475949AFF9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>